<commit_message>
ADD Table Exam; v:0.2.06
--> CHG everything from "Grade" to "Exam"
--> CHG FragmentExam to display all Exam for this year
--> ADD AddEditExam to add/edit Exam
--> ADD ExamSubjectYearExamtype (mergedEntity)
   -> contains: Exam, Subject, Year and Examtype
--> ADD getAllExamtypeList() to Examtype
--> ADD getAllSubjectList() to Subject
--> ADD Database initialization to MainActivity

Signed-off-by: rafi0101 <r-github@ebner-sachrang.de>
</commit_message>
<xml_diff>
--- a/ER_Database.xlsx
+++ b/ER_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raphael\AndroidStudioProjects\Stundenplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47A7C45-1AF3-48B3-85B0-A2F04235AF9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E58874-F3A6-4D86-879A-4590F3699795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74F2640E-B4BD-4A1B-82F4-218DA6BD8E14}"/>
+    <workbookView xWindow="28680" yWindow="1425" windowWidth="21840" windowHeight="13140" xr2:uid="{74F2640E-B4BD-4A1B-82F4-218DA6BD8E14}"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="2" r:id="rId1"/>
@@ -211,21 +211,12 @@
     <t>EID (PK)</t>
   </si>
   <si>
-    <t>EName</t>
-  </si>
-  <si>
     <t>E_SID (FK)</t>
   </si>
   <si>
     <t>EGrade</t>
   </si>
   <si>
-    <t>EWeighting</t>
-  </si>
-  <si>
-    <t>EDate</t>
-  </si>
-  <si>
     <t>E_ETID (FK)</t>
   </si>
   <si>
@@ -290,6 +281,15 @@
   </si>
   <si>
     <t>SET_YID (FK)</t>
+  </si>
+  <si>
+    <t>EDateYear</t>
+  </si>
+  <si>
+    <t>EDateMonth</t>
+  </si>
+  <si>
+    <t>EDateDay</t>
   </si>
 </sst>
 </file>
@@ -517,15 +517,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>87924</xdr:colOff>
+      <xdr:colOff>80597</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>43962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>102577</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>102577</xdr:rowOff>
+      <xdr:colOff>102578</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -540,8 +540,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5374299" y="3472962"/>
-          <a:ext cx="776653" cy="820615"/>
+          <a:off x="5370635" y="3472962"/>
+          <a:ext cx="783981" cy="615461"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1191,7 +1191,7 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="2633870" y="4671392"/>
-          <a:ext cx="5679385" cy="1391478"/>
+          <a:ext cx="5687229" cy="1391478"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2471,8 +2471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDA4289-FBD5-4D2F-9C66-D094E9CA6164}">
   <dimension ref="C3:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2551,7 +2551,7 @@
         <v>44</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>49</v>
@@ -2567,10 +2567,10 @@
         <v>48</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="I14" s="2"/>
       <c r="N14" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.25">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="I15" s="2"/>
       <c r="N15" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="O15" t="s">
         <v>12</v>
@@ -2618,18 +2618,18 @@
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>57</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D21" s="5">
         <v>1</v>
@@ -2644,41 +2644,41 @@
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>59</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="J24" s="6"/>
       <c r="K24" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L24" t="s">
         <v>12</v>
@@ -2687,24 +2687,24 @@
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F26" s="2" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F27" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
@@ -2716,20 +2716,19 @@
         <v>12</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="F29" s="2"/>
       <c r="K29" s="2"/>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I32" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="8:12" x14ac:dyDescent="0.25">
@@ -2737,11 +2736,11 @@
         <v>1</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L33" s="5">
         <v>1</v>
@@ -2749,16 +2748,16 @@
     </row>
     <row r="34" spans="8:12" x14ac:dyDescent="0.25">
       <c r="I34" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="8:12" x14ac:dyDescent="0.25">
       <c r="I35" s="2"/>
       <c r="K35" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="8:12" x14ac:dyDescent="0.25">

</xml_diff>